<commit_message>
alteração no nome da função dos processos
</commit_message>
<xml_diff>
--- a/server/excel/tags_filtradas.xlsx
+++ b/server/excel/tags_filtradas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:U17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,7 +543,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>PIT-1710.1</t>
+          <t>XV-1701.9</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -558,7 +558,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>PHS2-PR27-1701-FL.04 Rev. 00N</t>
+          <t>PHS2-PR27-1701-FL.01 Rev. 74I</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -568,27 +568,27 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ESFERA AUTOMÁTICA</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>1,5 kg/m3</t>
+          <t>1120 kg/m3</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>0,0186 cP</t>
+          <t>&lt;50 cP</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1,2</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -603,12 +603,12 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>15 - 30</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>-</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -626,8 +626,16 @@
           <t>(NOTA 1): CRESTIVO (A16003E); BIRK 25% (A25191A); BIRTEA; CRESTIVO DUO</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
       <c r="T2" t="inlineStr">
         <is>
           <t>9</t>
@@ -642,7 +650,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PIT-1710.2</t>
+          <t>XV-1702.10</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -652,12 +660,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>(NOTA 1)</t>
+          <t>BICICLOPIRONA EM PÓ</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>PHS2-PR27-1701-FL.04 Rev. 00N</t>
+          <t>PHS2-PR27-1701-FL.04 REV.00N</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -667,17 +675,17 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>GUILHOTINA AUTOMÁTICA</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>1,5 kg/m3</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>0,0186 cP</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -687,7 +695,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -722,7 +730,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>(NOTA 1): CRESTIVO (A16003E); BIRK 25% (A25191A); BIRTEA; CRESTIVO DUO</t>
+          <t>-</t>
         </is>
       </c>
       <c r="R3" t="inlineStr"/>
@@ -741,7 +749,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>PIT-1716.1</t>
+          <t>XV-1702.9</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -751,87 +759,1470 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>AR + TRAÇOS DE BICICLOPIRONA EM PÓ</t>
+          <t>(NOTA 1)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>PHS2-PR27-1701-FL.01 Rev. 74I</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>ESFERA AUTOMÁTICA</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>1120 kg/m3</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>&lt;50 cP</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>1,2</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>9 - 35</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>15 - 30</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>(NOTA 1): CRESTIVO (A16003E); BIRK 25% (A25191A); BIRTEA; CRESTIVO DUO</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>XV-1710.3</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>(NOTA 1)</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>PHS2-PR27-1701-FL.04 REV.00N</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>ESFERA AUTOMÁTICA</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>1120 kg/m³</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>&lt;50 cP</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>9 - 35</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>(NOTA 1): CRESTIVO (A16003E); BIRK 25% (A25191A); BIRTEA; CRESTIVO DUO</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>XV-1710.4</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>(NOTA 1)</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>PHS2-PR27-1701-FL.04 REV.00N</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>ESFERA AUTOMÁTICA</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>1120 kg/m³</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>&lt;50 cP</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>9 - 35</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>15 - 30</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>(NOTA 1): CRESTIVO (A16003E); BIRK 25% (A25191A); BIRTEA; CRESTIVO DUO</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>XV-1710.5</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>(NOTA 1)</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>PHS2-PR27-1701-FL.04 Rev. 00N</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>ATM</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>ESFERA AUTOMÁTICA</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>1120 kg/m3</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>&lt;50 cP</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>0,984</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
         <is>
           <t>9 - 35</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="L7" t="inlineStr">
         <is>
           <t>65</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
-      <c r="T4" t="inlineStr">
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>15 - 30</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>(NOTA 1): CRESTIVO (A16003E); BIRK 25% (A25191A); BIRTEA; CRESTIVO DUO</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
         <is>
           <t>9</t>
         </is>
       </c>
-      <c r="U4" t="inlineStr">
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>XV-1710.6</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>ÁGUA DE PROCESSO</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>PHS2-PR27-1701-FL.04 Rev. 00N</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>ESFERA AUTOMÁTICA</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>998 kg/m3</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>1 cP</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>9 - 35</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>1 - 6</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>(NOTA 1): CRESTIVO (A16003E); BIRK 25% (A25191A); BIRTEA; CRESTIVO DUO</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>XV-1710.7</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>ÁGUA DE PROCESSO</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>PHS2-PR27-1701-FL.04 Rev. 00N</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>ESFERA AUTOMÁTICA</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>998 kg/m3</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>1 cP</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>9 - 35</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>1 - 6</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>(NOTA 1): CRESTIVO (A16003E); BIRK 25% (A25191A); BIRTEA; CRESTIVO DUO</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>XV-1710.8</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>AR + VAPOR DA FASE LÍQUIDA DE REAÇÃO (NOTA 1)</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>PHS2-PR27-1701-FL.04 Rev. 00N</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>GUILHOTINA AUTOMÁTICA</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>1,5 kg/m3</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>0,0186 cP</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>9 - 35</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>(NOTA 1): CRESTIVO (A16003E); BIRK 25% (A25191A); BIRTEA; CRESTIVO DUO</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="inlineStr"/>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>XV-1715.1</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>(NOTA 1)</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>PHS2-PR27-1701-FL.01 Rev. 74I</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>ESFERA AUTOMÁTICA</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>1120 kg/m³</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>&lt;50 cP</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>3,00</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>6,00</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>9 - 35</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>15 - 30</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>(NOTA 1): CRESTIVO (A16003E); BIRK 25% (A25191A); BIRTEA; CRESTIVO DUO</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>XV-1715.2</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>(NOTA 1)</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>PHS2-PR27-1701-FL.01 Rev. 74I</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>ESFERA AUTOMÁTICA</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>1120 kg/m³</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>&lt;50 cP</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>3,00</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>6,00</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>9 - 35</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>15 - 30</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>(NOTA 1): CRESTIVO (A16003E); BIRK 25% (A25191A); BIRTEA; CRESTIVO DUO</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>XV-1715.3</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>(NOTA 1)</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>PHS2-PR27-1701-FL.01 Rev. 74I</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>ESFERA AUTOMÁTICA</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>1120 kg/m³</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>&lt;50 cP</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>3,00</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>6,00</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>9 - 35</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>15 - 30</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>(NOTA 1): CRESTIVO (A16003E); BIRK 25% (A25191A); BIRTEA; CRESTIVO DUO</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>XV-1715.4</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>(NOTA 1)</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>PHS2-PR27-1701-FL.01 Rev. 74I</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>ESFERA AUTOMÁTICA</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>1120 kg/m³</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>&lt;50 cP</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>3,00</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>6,00</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>9 - 35</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>15 - 30</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>(NOTA 1): CRESTIVO (A16003E); BIRK 25% (A25191A); BIRTEA; CRESTIVO DUO</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>XV-1715.5</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>(NOTA 1)</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>PHS2-PR27-1701-FL.01 Rev. 74I</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>ESFERA AUTOMÁTICA</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>1120 kg/m³</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>&lt;50 cP</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>3,00</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>6,00</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>9 - 35</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>15 - 30</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>(NOTA 1): CRESTIVO (A16003E); BIRK 25% (A25191A); BIRTEA; CRESTIVO DUO</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>XV-1715.6</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>(NOTA 1)</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>PHS2-PR27-1701-FL.01 Rev. 74I</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>ESFERA AUTOMÁTICA</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>1120 kg/m³</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>&lt;50 cP</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>3,00</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>6,00</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>9 - 35</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>15 - 30</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>(NOTA 1): CRESTIVO (A16003E); BIRK 25% (A25191A); BIRTEA; CRESTIVO DUO</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>XV-1715.7</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>(NOTA 1)</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>PHS2-PR27-1701-FL.01 Rev. 74I</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>ESFERA AUTOMÁTICA</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>1120 kg/m³</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>&lt;50 cP</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>3,00</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>6,00</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>9 - 35</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>15 - 30</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>(NOTA 1): CRESTIVO (A16003E); BIRK 25% (A25191A); BIRTEA; CRESTIVO DUO</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr">
         <is>
           <t>35</t>
         </is>

</xml_diff>

<commit_message>
CONECTADO NO DOCKER 🎉🎉🎉
</commit_message>
<xml_diff>
--- a/server/excel/tags_filtradas.xlsx
+++ b/server/excel/tags_filtradas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U13"/>
+  <dimension ref="A1:U17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,7 +543,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ZS-1702.1</t>
+          <t>XV-1701.9</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -553,12 +553,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>(NOTA 1)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>PHS2-PR27-1701-FL.04 Rev. 00N</t>
+          <t>PHS2-PR27-1701-FL.01 Rev. 74I</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -568,27 +568,27 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ESFERA AUTOMÁTICA</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1120 kg/m3</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>&lt;50 cP</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>ATM</t>
+          <t>1,2</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -598,12 +598,12 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>65</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>15 - 30</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -621,9 +621,21 @@
           <t>-</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>(NOTA 1): CRESTIVO (A16003E); BIRK 25% (A25191A); BIRTEA; CRESTIVO DUO</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
       <c r="T2" t="inlineStr">
         <is>
           <t>9</t>
@@ -638,7 +650,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ZS-1710.1</t>
+          <t>XV-1702.10</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -648,12 +660,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>BICICLOPIRONA EM PÓ</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>PHS2-PR27-1701-FL.04 Rev. 00N</t>
+          <t>PHS2-PR27-1701-FL.04 REV.00N</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -663,7 +675,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>GUILHOTINA AUTOMÁTICA</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -678,12 +690,12 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>ATM</t>
+          <t>-</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -693,7 +705,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>65</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -703,7 +715,7 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>F</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -716,7 +728,11 @@
           <t>-</t>
         </is>
       </c>
-      <c r="Q3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr">
@@ -733,7 +749,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ZS-1710.2</t>
+          <t>XV-1702.9</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -743,12 +759,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>(NOTA 1)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>PHS2-PR27-1701-FL.04 Rev. 00N</t>
+          <t>PHS2-PR27-1701-FL.01 Rev. 74I</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -758,27 +774,27 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ESFERA AUTOMÁTICA</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1120 kg/m3</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>&lt;50 cP</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>ATM</t>
+          <t>1,2</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -788,12 +804,12 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>65</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>15 - 30</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -811,9 +827,21 @@
           <t>-</t>
         </is>
       </c>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>(NOTA 1): CRESTIVO (A16003E); BIRK 25% (A25191A); BIRTEA; CRESTIVO DUO</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
       <c r="T4" t="inlineStr">
         <is>
           <t>9</t>
@@ -828,7 +856,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ZS-1710A.2</t>
+          <t>XV-1710.3</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -838,12 +866,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>(NOTA 1)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>PHS2-PR27-1701-FL.04 Rev. 00N</t>
+          <t>PHS2-PR27-1701-FL.04 REV.00N</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -853,27 +881,27 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ESFERA AUTOMÁTICA</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1120 kg/m³</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>&lt;50 cP</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>ATM</t>
+          <t>-</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -883,17 +911,15 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="M5" t="n">
+        <v>15</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>F</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -906,7 +932,11 @@
           <t>-</t>
         </is>
       </c>
-      <c r="Q5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>(NOTA 1): CRESTIVO (A16003E); BIRK 25% (A25191A); BIRTEA; CRESTIVO DUO</t>
+        </is>
+      </c>
       <c r="R5" t="inlineStr"/>
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr">
@@ -923,7 +953,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ZS-1710A.3</t>
+          <t>XV-1710.4</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -933,12 +963,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>(NOTA 1)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>PHS2-PR27-1701-FL.04 Rev. 00N</t>
+          <t>PHS2-PR27-1701-FL.04 REV.00N</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -948,27 +978,27 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ESFERA AUTOMÁTICA</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1120 kg/m³</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>&lt;50 cP</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>ATM</t>
+          <t>-</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -978,17 +1008,17 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>65</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>15 - 30</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>F</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
@@ -1001,9 +1031,21 @@
           <t>-</t>
         </is>
       </c>
-      <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="inlineStr"/>
-      <c r="S6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>(NOTA 1): CRESTIVO (A16003E); BIRK 25% (A25191A); BIRTEA; CRESTIVO DUO</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
       <c r="T6" t="inlineStr">
         <is>
           <t>9</t>
@@ -1018,17 +1060,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ZS-1710A.4</t>
+          <t>XV-1710.5</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>3"</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>(NOTA 1)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1043,27 +1085,27 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ESFERA AUTOMÁTICA</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1120 kg/m3</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>&lt;50 cP</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>ATM</t>
+          <t>0,984</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -1073,17 +1115,17 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>65</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>15 - 30</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>F</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
@@ -1096,9 +1138,21 @@
           <t>-</t>
         </is>
       </c>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr"/>
-      <c r="S7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>(NOTA 1): CRESTIVO (A16003E); BIRK 25% (A25191A); BIRTEA; CRESTIVO DUO</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
       <c r="T7" t="inlineStr">
         <is>
           <t>9</t>
@@ -1113,7 +1167,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ZS-1715</t>
+          <t>XV-1710.6</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1123,12 +1177,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ÁGUA DE PROCESSO</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>PHS2-PR27-1701-FL.01 Rev. 74I</t>
+          <t>PHS2-PR27-1701-FL.04 Rev. 00N</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1138,27 +1192,27 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>FIM DE CURSO</t>
+          <t>ESFERA AUTOMÁTICA</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>998 kg/m3</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1 cP</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>ATM</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -1173,12 +1227,12 @@
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1 - 6</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>F</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
@@ -1193,11 +1247,19 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R8" t="inlineStr"/>
-      <c r="S8" t="inlineStr"/>
+          <t>(NOTA 1): CRESTIVO (A16003E); BIRK 25% (A25191A); BIRTEA; CRESTIVO DUO</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
       <c r="T8" t="inlineStr">
         <is>
           <t>9</t>
@@ -1212,7 +1274,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ZS-1715.1</t>
+          <t>XV-1710.7</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1222,12 +1284,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>ÁGUA DE PROCESSO</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>PHS2-PR27-1701-FL.01 Rev. 74I</t>
+          <t>PHS2-PR27-1701-FL.04 Rev. 00N</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1237,27 +1299,27 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>FIM DE CURSO</t>
+          <t>ESFERA AUTOMÁTICA</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>998 kg/m3</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1 cP</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>ATM</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>3</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1272,12 +1334,12 @@
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1 - 6</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>F</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
@@ -1292,11 +1354,19 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R9" t="inlineStr"/>
-      <c r="S9" t="inlineStr"/>
+          <t>(NOTA 1): CRESTIVO (A16003E); BIRK 25% (A25191A); BIRTEA; CRESTIVO DUO</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
       <c r="T9" t="inlineStr">
         <is>
           <t>9</t>
@@ -1311,7 +1381,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ZS-1715.2</t>
+          <t>XV-1710.8</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1321,12 +1391,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AR + VAPOR DA FASE LÍQUIDA DE REAÇÃO (NOTA 1)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>PHS2-PR27-1701-FL.01 Rev. 74I</t>
+          <t>PHS2-PR27-1701-FL.04 Rev. 00N</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1336,22 +1406,22 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>FIM DE CURSO</t>
+          <t>GUILHOTINA AUTOMÁTICA</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1,5 kg/m3</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0,0186 cP</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>ATM</t>
+          <t>-</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -1376,7 +1446,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>A</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -1391,7 +1461,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>(NOTA 1): CRESTIVO (A16003E); BIRK 25% (A25191A); BIRTEA; CRESTIVO DUO</t>
         </is>
       </c>
       <c r="R10" t="inlineStr"/>
@@ -1410,7 +1480,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ZS-1715.5</t>
+          <t>XV-1715.1</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1420,7 +1490,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>(NOTA 1)</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1435,27 +1505,27 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>FIM DE CURSO</t>
+          <t>ESFERA AUTOMÁTICA</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1120 kg/m³</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>&lt;50 cP</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>ATM</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1470,7 +1540,7 @@
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>15 - 30</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
@@ -1490,11 +1560,19 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R11" t="inlineStr"/>
-      <c r="S11" t="inlineStr"/>
+          <t>(NOTA 1): CRESTIVO (A16003E); BIRK 25% (A25191A); BIRTEA; CRESTIVO DUO</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
       <c r="T11" t="inlineStr">
         <is>
           <t>9</t>
@@ -1509,7 +1587,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ZS-1715.6</t>
+          <t>XV-1715.2</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1519,7 +1597,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>(NOTA 1)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1534,27 +1612,27 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>FIM DE CURSO</t>
+          <t>ESFERA AUTOMÁTICA</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1120 kg/m³</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>&lt;50 cP</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>ATM</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1569,7 +1647,7 @@
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>15 - 30</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
@@ -1589,11 +1667,19 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R12" t="inlineStr"/>
-      <c r="S12" t="inlineStr"/>
+          <t>(NOTA 1): CRESTIVO (A16003E); BIRK 25% (A25191A); BIRTEA; CRESTIVO DUO</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
       <c r="T12" t="inlineStr">
         <is>
           <t>9</t>
@@ -1608,7 +1694,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ZS-1715.7</t>
+          <t>XV-1715.3</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1618,7 +1704,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>(NOTA 1)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1633,42 +1719,42 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>FIM DE CURSO</t>
+          <t>ESFERA AUTOMÁTICA</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1120 kg/m³</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>&lt;50 cP</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>ATM</t>
+          <t>3,00</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>6,00</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>10 - 35</t>
+          <t>9 - 35</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>66</t>
+          <t>65</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>15 - 30</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
@@ -1688,17 +1774,453 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R13" t="inlineStr"/>
-      <c r="S13" t="inlineStr"/>
+          <t>(NOTA 1): CRESTIVO (A16003E); BIRK 25% (A25191A); BIRTEA; CRESTIVO DUO</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>9</t>
         </is>
       </c>
       <c r="U13" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>XV-1715.4</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>(NOTA 1)</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>PHS2-PR27-1701-FL.01 Rev. 74I</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>ESFERA AUTOMÁTICA</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>1120 kg/m³</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>&lt;50 cP</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>3,00</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>6,00</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>9 - 35</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>15 - 30</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>(NOTA 1): CRESTIVO (A16003E); BIRK 25% (A25191A); BIRTEA; CRESTIVO DUO</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>XV-1715.5</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>(NOTA 1)</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>PHS2-PR27-1701-FL.01 Rev. 74I</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>ESFERA AUTOMÁTICA</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>1120 kg/m³</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>&lt;50 cP</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>3,00</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>6,00</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>9 - 35</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>15 - 30</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>(NOTA 1): CRESTIVO (A16003E); BIRK 25% (A25191A); BIRTEA; CRESTIVO DUO</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>XV-1715.6</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>(NOTA 1)</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>PHS2-PR27-1701-FL.01 Rev. 74I</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>ESFERA AUTOMÁTICA</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>1120 kg/m³</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>&lt;50 cP</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>3,00</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>6,00</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>9 - 35</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>15 - 30</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>(NOTA 1): CRESTIVO (A16003E); BIRK 25% (A25191A); BIRTEA; CRESTIVO DUO</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>XV-1715.7</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>(NOTA 1)</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>PHS2-PR27-1701-FL.01 Rev. 74I</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>ESFERA AUTOMÁTICA</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>1120 kg/m³</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>&lt;50 cP</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>3,00</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>6,00</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>9 - 35</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>15 - 30</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>(NOTA 1): CRESTIVO (A16003E); BIRK 25% (A25191A); BIRTEA; CRESTIVO DUO</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr">
         <is>
           <t>35</t>
         </is>

</xml_diff>